<commit_message>
Modified Supplementary materials 2-3 by adding the interpretable coefficients and 95% CIs
</commit_message>
<xml_diff>
--- a/data/Supplementary Material 2.xlsx
+++ b/data/Supplementary Material 2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve">income_group</t>
   </si>
@@ -59,6 +59,21 @@
     <t xml:space="preserve">adjusted_p_value</t>
   </si>
   <si>
+    <t xml:space="preserve">effect_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effect_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ci_lower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ci_upper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effect_size_for_plotting</t>
+  </si>
+  <si>
     <t xml:space="preserve">HIC</t>
   </si>
   <si>
@@ -71,6 +86,9 @@
     <t xml:space="preserve">beta</t>
   </si>
   <si>
+    <t xml:space="preserve">OR</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIC</t>
   </si>
   <si>
@@ -86,6 +104,9 @@
     <t xml:space="preserve">linear</t>
   </si>
   <si>
+    <t xml:space="preserve">Coefficient</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hospital.beds..per.1.000.people.</t>
   </si>
   <si>
@@ -123,6 +144,9 @@
   </si>
   <si>
     <t xml:space="preserve">negbin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRR</t>
   </si>
   <si>
     <t xml:space="preserve">poisson</t>
@@ -509,22 +533,37 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D2" t="n">
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F2" t="n">
         <v>0.00050290169030051</v>
@@ -552,22 +591,37 @@
       <c r="O2" t="n">
         <v>0.598035678322598</v>
       </c>
+      <c r="P2" t="n">
+        <v>1.00050302816656</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.999071365892342</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1.00193674200279</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.000503028166556341</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D3" t="n">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F3" t="n">
         <v>0.0121456509076672</v>
@@ -595,22 +649,37 @@
       <c r="O3" t="n">
         <v>0.096935456978826</v>
       </c>
+      <c r="P3" t="n">
+        <v>1.01221970884924</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.99937519819824</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1.02522930409926</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.0122197088492424</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D4" t="n">
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F4" t="n">
         <v>0.00151612816004284</v>
@@ -638,22 +707,37 @@
       <c r="O4" t="n">
         <v>0.236702348396164</v>
       </c>
+      <c r="P4" t="n">
+        <v>1.0015172780634</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.999379279099262</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1.00365985090621</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.00151727806340185</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D5" t="n">
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F5" t="n">
         <v>0.00407933815045251</v>
@@ -681,22 +765,37 @@
       <c r="O5" t="n">
         <v>0.000176872933400634</v>
       </c>
+      <c r="P5" t="n">
+        <v>1.00408766997592</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>24</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1.00212398669947</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1.00605520113153</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.00408766997591736</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D6" t="n">
         <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F6" t="n">
         <v>-0.000234283676139777</v>
@@ -726,22 +825,37 @@
       <c r="O6" t="n">
         <v>0.971533429267544</v>
       </c>
+      <c r="P6" t="n">
+        <v>-0.000234283676139777</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>30</v>
+      </c>
+      <c r="R6" t="n">
+        <v>-0.0052240220143095</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.00475545466202994</v>
+      </c>
+      <c r="T6" t="n">
+        <v>-0.000234283676139777</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D7" t="n">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F7" t="n">
         <v>-0.485651428571429</v>
@@ -771,22 +885,37 @@
       <c r="O7" t="n">
         <v>0.433527414498355</v>
       </c>
+      <c r="P7" t="n">
+        <v>-0.485651428571429</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R7" t="n">
+        <v>-1.71089028438649</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.739587427243636</v>
+      </c>
+      <c r="T7" t="n">
+        <v>-0.485651428571429</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D8" t="n">
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F8" t="n">
         <v>-0.0784509930154872</v>
@@ -816,22 +945,37 @@
       <c r="O8" t="n">
         <v>0.0637299936420243</v>
       </c>
+      <c r="P8" t="n">
+        <v>-0.0784509930154872</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R8" t="n">
+        <v>-0.149777684265559</v>
+      </c>
+      <c r="S8" t="n">
+        <v>-0.00712430176541506</v>
+      </c>
+      <c r="T8" t="n">
+        <v>-0.0784509930154872</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D9" t="n">
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F9" t="n">
         <v>0.0192510812482215</v>
@@ -861,22 +1005,37 @@
       <c r="O9" t="n">
         <v>0.0952396737667322</v>
       </c>
+      <c r="P9" t="n">
+        <v>0.0192510812482215</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>30</v>
+      </c>
+      <c r="R9" t="n">
+        <v>-0.000854094380182684</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.0393562568766257</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.0192510812482215</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D10" t="n">
         <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F10" t="n">
         <v>-0.0192452271883566</v>
@@ -906,22 +1065,37 @@
       <c r="O10" t="n">
         <v>0.000000188418359114931</v>
       </c>
+      <c r="P10" t="n">
+        <v>-0.0192452271883566</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>30</v>
+      </c>
+      <c r="R10" t="n">
+        <v>-0.0237112027563919</v>
+      </c>
+      <c r="S10" t="n">
+        <v>-0.0147792516203213</v>
+      </c>
+      <c r="T10" t="n">
+        <v>-0.0192452271883566</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D11" t="n">
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F11" t="n">
         <v>0.166211004273504</v>
@@ -951,22 +1125,37 @@
       <c r="O11" t="n">
         <v>0.00357797061053061</v>
       </c>
+      <c r="P11" t="n">
+        <v>0.166211004273504</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>30</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.122506938284234</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.209915070262774</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.166211004273504</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D12" t="n">
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F12" t="n">
         <v>0.0153207000478395</v>
@@ -996,22 +1185,37 @@
       <c r="O12" t="n">
         <v>0.0771768479261046</v>
       </c>
+      <c r="P12" t="n">
+        <v>0.0153207000478395</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>30</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.000606666862020915</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.0300347332336581</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.0153207000478395</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D13" t="n">
         <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F13" t="n">
         <v>-0.00443220123984373</v>
@@ -1041,22 +1245,37 @@
       <c r="O13" t="n">
         <v>0.379813427312861</v>
       </c>
+      <c r="P13" t="n">
+        <v>-0.00443220123984373</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>30</v>
+      </c>
+      <c r="R13" t="n">
+        <v>-0.0127776333193477</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.00391323083966027</v>
+      </c>
+      <c r="T13" t="n">
+        <v>-0.00443220123984373</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D14" t="n">
         <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F14" t="n">
         <v>-0.0246897233096417</v>
@@ -1086,22 +1305,37 @@
       <c r="O14" t="n">
         <v>0.00000597133949789282</v>
       </c>
+      <c r="P14" t="n">
+        <v>-0.0246897233096417</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>30</v>
+      </c>
+      <c r="R14" t="n">
+        <v>-0.0323973389256636</v>
+      </c>
+      <c r="S14" t="n">
+        <v>-0.0169821076936198</v>
+      </c>
+      <c r="T14" t="n">
+        <v>-0.0246897233096417</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D15" t="n">
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F15" t="n">
         <v>-1.15714285714286</v>
@@ -1131,22 +1365,37 @@
       <c r="O15" t="n">
         <v>0.207017182227322</v>
       </c>
+      <c r="P15" t="n">
+        <v>-1.15714285714286</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>30</v>
+      </c>
+      <c r="R15" t="n">
+        <v>-2.8866512726797</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.572365558393978</v>
+      </c>
+      <c r="T15" t="n">
+        <v>-1.15714285714286</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D16" t="n">
         <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F16" t="n">
         <v>-0.392836926814455</v>
@@ -1176,22 +1425,37 @@
       <c r="O16" t="n">
         <v>0.0106986211041426</v>
       </c>
+      <c r="P16" t="n">
+        <v>-0.392836926814455</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>30</v>
+      </c>
+      <c r="R16" t="n">
+        <v>-0.643766421985998</v>
+      </c>
+      <c r="S16" t="n">
+        <v>-0.141907431642912</v>
+      </c>
+      <c r="T16" t="n">
+        <v>-0.392836926814455</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D17" t="n">
         <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F17" t="n">
         <v>-0.150629988341853</v>
@@ -1221,22 +1485,37 @@
       <c r="O17" t="n">
         <v>0.00002523616933698</v>
       </c>
+      <c r="P17" t="n">
+        <v>-0.150629988341853</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>30</v>
+      </c>
+      <c r="R17" t="n">
+        <v>-0.200060513422762</v>
+      </c>
+      <c r="S17" t="n">
+        <v>-0.101199463260944</v>
+      </c>
+      <c r="T17" t="n">
+        <v>-0.150629988341853</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D18" t="n">
         <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F18" t="n">
         <v>-0.0478765969215814</v>
@@ -1266,22 +1545,37 @@
       <c r="O18" t="n">
         <v>0.00000597133949789282</v>
       </c>
+      <c r="P18" t="n">
+        <v>-0.0478765969215814</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>30</v>
+      </c>
+      <c r="R18" t="n">
+        <v>-0.0630840038597627</v>
+      </c>
+      <c r="S18" t="n">
+        <v>-0.0326691899834</v>
+      </c>
+      <c r="T18" t="n">
+        <v>-0.0478765969215814</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D19" t="n">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F19" t="n">
         <v>-7.48628571428572</v>
@@ -1311,22 +1605,37 @@
       <c r="O19" t="n">
         <v>0.251307881262644</v>
       </c>
+      <c r="P19" t="n">
+        <v>-7.48628571428572</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>30</v>
+      </c>
+      <c r="R19" t="n">
+        <v>-20.2778834838482</v>
+      </c>
+      <c r="S19" t="n">
+        <v>5.30531205527673</v>
+      </c>
+      <c r="T19" t="n">
+        <v>-7.48628571428572</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D20" t="n">
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F20" t="n">
         <v>-1.53991223808078</v>
@@ -1356,22 +1665,37 @@
       <c r="O20" t="n">
         <v>0.0107778393160598</v>
       </c>
+      <c r="P20" t="n">
+        <v>-1.53991223808078</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>30</v>
+      </c>
+      <c r="R20" t="n">
+        <v>-2.53075449077423</v>
+      </c>
+      <c r="S20" t="n">
+        <v>-0.549069985387333</v>
+      </c>
+      <c r="T20" t="n">
+        <v>-1.53991223808078</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D21" t="n">
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F21" t="n">
         <v>-0.37724167115057</v>
@@ -1401,22 +1725,37 @@
       <c r="O21" t="n">
         <v>0.000037914661692857</v>
       </c>
+      <c r="P21" t="n">
+        <v>-0.37724167115057</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>30</v>
+      </c>
+      <c r="R21" t="n">
+        <v>-0.506928220262183</v>
+      </c>
+      <c r="S21" t="n">
+        <v>-0.247555122038957</v>
+      </c>
+      <c r="T21" t="n">
+        <v>-0.37724167115057</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D22" t="n">
         <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F22" t="n">
         <v>-0.0395017439568685</v>
@@ -1446,22 +1785,37 @@
       <c r="O22" t="n">
         <v>0.00000597133949789282</v>
       </c>
+      <c r="P22" t="n">
+        <v>-0.0395017439568685</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>30</v>
+      </c>
+      <c r="R22" t="n">
+        <v>-0.0521009622723575</v>
+      </c>
+      <c r="S22" t="n">
+        <v>-0.0269025256413795</v>
+      </c>
+      <c r="T22" t="n">
+        <v>-0.0395017439568685</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D23" t="n">
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F23" t="n">
         <v>-4.228</v>
@@ -1491,22 +1845,37 @@
       <c r="O23" t="n">
         <v>0.236702348396164</v>
       </c>
+      <c r="P23" t="n">
+        <v>-4.228</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>30</v>
+      </c>
+      <c r="R23" t="n">
+        <v>-11.1435435267189</v>
+      </c>
+      <c r="S23" t="n">
+        <v>2.68754352671891</v>
+      </c>
+      <c r="T23" t="n">
+        <v>-4.228</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D24" t="n">
         <v>19</v>
       </c>
       <c r="E24" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F24" t="n">
         <v>-0.973505314303066</v>
@@ -1536,22 +1905,37 @@
       <c r="O24" t="n">
         <v>0.0106986211041426</v>
       </c>
+      <c r="P24" t="n">
+        <v>-0.973505314303066</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>30</v>
+      </c>
+      <c r="R24" t="n">
+        <v>-1.59336394557363</v>
+      </c>
+      <c r="S24" t="n">
+        <v>-0.353646683032499</v>
+      </c>
+      <c r="T24" t="n">
+        <v>-0.973505314303066</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D25" t="n">
         <v>21</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F25" t="n">
         <v>-0.278906039817057</v>
@@ -1581,22 +1965,37 @@
       <c r="O25" t="n">
         <v>0.00002523616933698</v>
       </c>
+      <c r="P25" t="n">
+        <v>-0.278906039817057</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>30</v>
+      </c>
+      <c r="R25" t="n">
+        <v>-0.371155929041142</v>
+      </c>
+      <c r="S25" t="n">
+        <v>-0.186656150592972</v>
+      </c>
+      <c r="T25" t="n">
+        <v>-0.278906039817057</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D26" t="n">
         <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F26" t="n">
         <v>2.06597427559015</v>
@@ -1626,22 +2025,37 @@
       <c r="O26" t="n">
         <v>0.0771768479261046</v>
       </c>
+      <c r="P26" t="n">
+        <v>2.06597427559015</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>30</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.0596215635457549</v>
+      </c>
+      <c r="S26" t="n">
+        <v>4.07232698763455</v>
+      </c>
+      <c r="T26" t="n">
+        <v>2.06597427559015</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D27" t="n">
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F27" t="n">
         <v>0.00868844604845105</v>
@@ -1671,22 +2085,37 @@
       <c r="O27" t="n">
         <v>0.986945295107133</v>
       </c>
+      <c r="P27" t="n">
+        <v>0.00868844604845105</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>30</v>
+      </c>
+      <c r="R27" t="n">
+        <v>-1.54819172081079</v>
+      </c>
+      <c r="S27" t="n">
+        <v>1.5655686129077</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0.00868844604845105</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D28" t="n">
         <v>19</v>
       </c>
       <c r="E28" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F28" t="n">
         <v>0.556289127656581</v>
@@ -1716,22 +2145,37 @@
       <c r="O28" t="n">
         <v>0.535600125482955</v>
       </c>
+      <c r="P28" t="n">
+        <v>0.556289127656581</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>30</v>
+      </c>
+      <c r="R28" t="n">
+        <v>-0.896720088273793</v>
+      </c>
+      <c r="S28" t="n">
+        <v>2.00929834358696</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0.556289127656581</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D29" t="n">
         <v>21</v>
       </c>
       <c r="E29" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F29" t="n">
         <v>1.32670509864465</v>
@@ -1761,22 +2205,37 @@
       <c r="O29" t="n">
         <v>0.0777347325935286</v>
       </c>
+      <c r="P29" t="n">
+        <v>1.32670509864465</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>30</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0.018192166569631</v>
+      </c>
+      <c r="S29" t="n">
+        <v>2.63521803071967</v>
+      </c>
+      <c r="T29" t="n">
+        <v>1.32670509864465</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D30" t="n">
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F30" t="n">
         <v>-0.213896076876286</v>
@@ -1806,22 +2265,37 @@
       <c r="O30" t="n">
         <v>0.00000597133949789282</v>
       </c>
+      <c r="P30" t="n">
+        <v>-0.213896076876286</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>30</v>
+      </c>
+      <c r="R30" t="n">
+        <v>-0.282491789976186</v>
+      </c>
+      <c r="S30" t="n">
+        <v>-0.145300363776387</v>
+      </c>
+      <c r="T30" t="n">
+        <v>-0.213896076876286</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D31" t="n">
         <v>6</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F31" t="n">
         <v>-4.89105714285715</v>
@@ -1851,22 +2325,37 @@
       <c r="O31" t="n">
         <v>0.752581017130684</v>
       </c>
+      <c r="P31" t="n">
+        <v>-4.89105714285715</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>30</v>
+      </c>
+      <c r="R31" t="n">
+        <v>-33.3834592149629</v>
+      </c>
+      <c r="S31" t="n">
+        <v>23.6013449292486</v>
+      </c>
+      <c r="T31" t="n">
+        <v>-4.89105714285715</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D32" t="n">
         <v>19</v>
       </c>
       <c r="E32" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F32" t="n">
         <v>-3.46640658366231</v>
@@ -1896,22 +2385,37 @@
       <c r="O32" t="n">
         <v>0.027717272674005</v>
       </c>
+      <c r="P32" t="n">
+        <v>-3.46640658366231</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>30</v>
+      </c>
+      <c r="R32" t="n">
+        <v>-6.08082234238711</v>
+      </c>
+      <c r="S32" t="n">
+        <v>-0.85199082493751</v>
+      </c>
+      <c r="T32" t="n">
+        <v>-3.46640658366231</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D33" t="n">
         <v>21</v>
       </c>
       <c r="E33" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F33" t="n">
         <v>-0.96643513103994</v>
@@ -1941,22 +2445,37 @@
       <c r="O33" t="n">
         <v>0.000154061088166498</v>
       </c>
+      <c r="P33" t="n">
+        <v>-0.96643513103994</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>30</v>
+      </c>
+      <c r="R33" t="n">
+        <v>-1.34378187344785</v>
+      </c>
+      <c r="S33" t="n">
+        <v>-0.589088388632031</v>
+      </c>
+      <c r="T33" t="n">
+        <v>-0.96643513103994</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D34" t="n">
         <v>29</v>
       </c>
       <c r="E34" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F34" t="n">
         <v>-0.414194687025802</v>
@@ -1986,22 +2505,37 @@
       <c r="O34" t="n">
         <v>0.0000234497720353126</v>
       </c>
+      <c r="P34" t="n">
+        <v>-0.414194687025802</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>30</v>
+      </c>
+      <c r="R34" t="n">
+        <v>-0.560066599126072</v>
+      </c>
+      <c r="S34" t="n">
+        <v>-0.268322774925532</v>
+      </c>
+      <c r="T34" t="n">
+        <v>-0.414194687025802</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D35" t="n">
         <v>6</v>
       </c>
       <c r="E35" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F35" t="n">
         <v>-4.60522857142856</v>
@@ -2031,22 +2565,37 @@
       <c r="O35" t="n">
         <v>0.792372230544143</v>
       </c>
+      <c r="P35" t="n">
+        <v>-4.60522857142856</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>30</v>
+      </c>
+      <c r="R35" t="n">
+        <v>-39.9414112412178</v>
+      </c>
+      <c r="S35" t="n">
+        <v>30.7309540983607</v>
+      </c>
+      <c r="T35" t="n">
+        <v>-4.60522857142856</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D36" t="n">
         <v>19</v>
       </c>
       <c r="E36" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F36" t="n">
         <v>-2.75304018220467</v>
@@ -2076,22 +2625,37 @@
       <c r="O36" t="n">
         <v>0.0547983570681985</v>
       </c>
+      <c r="P36" t="n">
+        <v>-2.75304018220467</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>30</v>
+      </c>
+      <c r="R36" t="n">
+        <v>-5.16022908381564</v>
+      </c>
+      <c r="S36" t="n">
+        <v>-0.345851280593704</v>
+      </c>
+      <c r="T36" t="n">
+        <v>-2.75304018220467</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D37" t="n">
         <v>21</v>
       </c>
       <c r="E37" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F37" t="n">
         <v>-1.27643151102871</v>
@@ -2121,22 +2685,37 @@
       <c r="O37" t="n">
         <v>0.000328691078341222</v>
       </c>
+      <c r="P37" t="n">
+        <v>-1.27643151102871</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>30</v>
+      </c>
+      <c r="R37" t="n">
+        <v>-1.81883400561205</v>
+      </c>
+      <c r="S37" t="n">
+        <v>-0.734029016445371</v>
+      </c>
+      <c r="T37" t="n">
+        <v>-1.27643151102871</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D38" t="n">
         <v>24</v>
       </c>
       <c r="E38" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F38" t="n">
         <v>2.06597427559015</v>
@@ -2166,22 +2745,37 @@
       <c r="O38" t="n">
         <v>0.0771768479261046</v>
       </c>
+      <c r="P38" t="n">
+        <v>2.06597427559015</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>30</v>
+      </c>
+      <c r="R38" t="n">
+        <v>0.0596215635457549</v>
+      </c>
+      <c r="S38" t="n">
+        <v>4.07232698763455</v>
+      </c>
+      <c r="T38" t="n">
+        <v>2.06597427559015</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D39" t="n">
         <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F39" t="n">
         <v>0.00868844604845105</v>
@@ -2211,22 +2805,37 @@
       <c r="O39" t="n">
         <v>0.986945295107133</v>
       </c>
+      <c r="P39" t="n">
+        <v>0.00868844604845105</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>30</v>
+      </c>
+      <c r="R39" t="n">
+        <v>-1.54819172081079</v>
+      </c>
+      <c r="S39" t="n">
+        <v>1.5655686129077</v>
+      </c>
+      <c r="T39" t="n">
+        <v>0.00868844604845105</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D40" t="n">
         <v>19</v>
       </c>
       <c r="E40" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F40" t="n">
         <v>0.556289127656581</v>
@@ -2256,22 +2865,37 @@
       <c r="O40" t="n">
         <v>0.535600125482955</v>
       </c>
+      <c r="P40" t="n">
+        <v>0.556289127656581</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>30</v>
+      </c>
+      <c r="R40" t="n">
+        <v>-0.896720088273793</v>
+      </c>
+      <c r="S40" t="n">
+        <v>2.00929834358696</v>
+      </c>
+      <c r="T40" t="n">
+        <v>0.556289127656581</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D41" t="n">
         <v>21</v>
       </c>
       <c r="E41" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F41" t="n">
         <v>1.32670509864465</v>
@@ -2301,22 +2925,37 @@
       <c r="O41" t="n">
         <v>0.0777347325935286</v>
       </c>
+      <c r="P41" t="n">
+        <v>1.32670509864465</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>30</v>
+      </c>
+      <c r="R41" t="n">
+        <v>0.018192166569631</v>
+      </c>
+      <c r="S41" t="n">
+        <v>2.63521803071967</v>
+      </c>
+      <c r="T41" t="n">
+        <v>1.32670509864465</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D42" t="n">
         <v>20</v>
       </c>
       <c r="E42" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F42" t="n">
         <v>0.00100926385492478</v>
@@ -2344,22 +2983,37 @@
       <c r="O42" t="n">
         <v>0.760872650446978</v>
       </c>
+      <c r="P42" t="n">
+        <v>1.00100977333307</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>24</v>
+      </c>
+      <c r="R42" t="n">
+        <v>0.996230796038467</v>
+      </c>
+      <c r="S42" t="n">
+        <v>1.00581167566079</v>
+      </c>
+      <c r="T42" t="n">
+        <v>0.00100977333307406</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D43" t="n">
         <v>5</v>
       </c>
       <c r="E43" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F43" t="n">
         <v>-0.0162220745373905</v>
@@ -2387,22 +3041,37 @@
       <c r="O43" t="n">
         <v>0.730211460949644</v>
       </c>
+      <c r="P43" t="n">
+        <v>0.983908794701307</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>24</v>
+      </c>
+      <c r="R43" t="n">
+        <v>0.921787712396936</v>
+      </c>
+      <c r="S43" t="n">
+        <v>1.0502163386115</v>
+      </c>
+      <c r="T43" t="n">
+        <v>-0.016091205298693</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D44" t="n">
         <v>18</v>
       </c>
       <c r="E44" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F44" t="n">
         <v>-0.0482803632218793</v>
@@ -2430,22 +3099,37 @@
       <c r="O44" t="n">
         <v>0.00040975497986939</v>
       </c>
+      <c r="P44" t="n">
+        <v>0.95286660087442</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>24</v>
+      </c>
+      <c r="R44" t="n">
+        <v>0.92965633483957</v>
+      </c>
+      <c r="S44" t="n">
+        <v>0.976656346044968</v>
+      </c>
+      <c r="T44" t="n">
+        <v>-0.0471333991255798</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C45" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D45" t="n">
         <v>19</v>
       </c>
       <c r="E45" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F45" t="n">
         <v>-0.0309543710413025</v>
@@ -2473,22 +3157,37 @@
       <c r="O45" t="n">
         <v>0.000000190218620898917</v>
       </c>
+      <c r="P45" t="n">
+        <v>0.969519810246148</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>24</v>
+      </c>
+      <c r="R45" t="n">
+        <v>0.959424235200978</v>
+      </c>
+      <c r="S45" t="n">
+        <v>0.979721616332555</v>
+      </c>
+      <c r="T45" t="n">
+        <v>-0.0304801897538516</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C46" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D46" t="n">
         <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F46" t="n">
         <v>-0.00119959285429965</v>
@@ -2516,22 +3215,37 @@
       <c r="O46" t="n">
         <v>0.695136253462987</v>
       </c>
+      <c r="P46" t="n">
+        <v>0.998801126369588</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>24</v>
+      </c>
+      <c r="R46" t="n">
+        <v>0.994528118986612</v>
+      </c>
+      <c r="S46" t="n">
+        <v>1.0030924928032</v>
+      </c>
+      <c r="T46" t="n">
+        <v>-0.00119887363041227</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D47" t="n">
         <v>5</v>
       </c>
       <c r="E47" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F47" t="n">
         <v>0.0318190450449162</v>
@@ -2559,22 +3273,37 @@
       <c r="O47" t="n">
         <v>0.433527414498355</v>
       </c>
+      <c r="P47" t="n">
+        <v>1.03233068305004</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>24</v>
+      </c>
+      <c r="R47" t="n">
+        <v>0.968061886188427</v>
+      </c>
+      <c r="S47" t="n">
+        <v>1.1008662301153</v>
+      </c>
+      <c r="T47" t="n">
+        <v>0.0323306830500389</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C48" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D48" t="n">
         <v>18</v>
       </c>
       <c r="E48" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F48" t="n">
         <v>-0.0376900007405774</v>
@@ -2602,22 +3331,37 @@
       <c r="O48" t="n">
         <v>0.000565737793683297</v>
       </c>
+      <c r="P48" t="n">
+        <v>0.963011427452829</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>24</v>
+      </c>
+      <c r="R48" t="n">
+        <v>0.944191904657698</v>
+      </c>
+      <c r="S48" t="n">
+        <v>0.982206058778851</v>
+      </c>
+      <c r="T48" t="n">
+        <v>-0.0369885725471715</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D49" t="n">
         <v>19</v>
       </c>
       <c r="E49" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F49" t="n">
         <v>-0.0227803195680817</v>
@@ -2645,22 +3389,37 @@
       <c r="O49" t="n">
         <v>0.00000165884708414809</v>
       </c>
+      <c r="P49" t="n">
+        <v>0.977477192800632</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>24</v>
+      </c>
+      <c r="R49" t="n">
+        <v>0.969350742872901</v>
+      </c>
+      <c r="S49" t="n">
+        <v>0.985671769966015</v>
+      </c>
+      <c r="T49" t="n">
+        <v>-0.0225228071993676</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C50" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D50" t="n">
         <v>30</v>
       </c>
       <c r="E50" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F50" t="n">
         <v>33712539.4408445</v>
@@ -2690,22 +3449,37 @@
       <c r="O50" t="n">
         <v>0.00931881644561653</v>
       </c>
+      <c r="P50" t="n">
+        <v>33712539.4408445</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>30</v>
+      </c>
+      <c r="R50" t="n">
+        <v>12192963.2890041</v>
+      </c>
+      <c r="S50" t="n">
+        <v>55232115.5926849</v>
+      </c>
+      <c r="T50" t="n">
+        <v>33712539.4408445</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B51" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C51" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D51" t="n">
         <v>6</v>
       </c>
       <c r="E51" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F51" t="n">
         <v>308170.14873164</v>
@@ -2735,22 +3509,37 @@
       <c r="O51" t="n">
         <v>0.971533429267544</v>
       </c>
+      <c r="P51" t="n">
+        <v>308170.14873164</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>30</v>
+      </c>
+      <c r="R51" t="n">
+        <v>-9836245.7366037</v>
+      </c>
+      <c r="S51" t="n">
+        <v>10452586.034067</v>
+      </c>
+      <c r="T51" t="n">
+        <v>308170.14873164</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B52" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C52" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D52" t="n">
         <v>20</v>
       </c>
       <c r="E52" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F52" t="n">
         <v>23025932.3298479</v>
@@ -2780,22 +3569,37 @@
       <c r="O52" t="n">
         <v>0.0541073673328307</v>
       </c>
+      <c r="P52" t="n">
+        <v>23025932.3298479</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>30</v>
+      </c>
+      <c r="R52" t="n">
+        <v>3071881.0976366</v>
+      </c>
+      <c r="S52" t="n">
+        <v>42979983.5620592</v>
+      </c>
+      <c r="T52" t="n">
+        <v>23025932.3298479</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C53" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D53" t="n">
         <v>22</v>
       </c>
       <c r="E53" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F53" t="n">
         <v>42486481.0119743</v>
@@ -2825,22 +3629,37 @@
       <c r="O53" t="n">
         <v>0.00018315651216372</v>
       </c>
+      <c r="P53" t="n">
+        <v>42486481.0119743</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>30</v>
+      </c>
+      <c r="R53" t="n">
+        <v>25267904.4237443</v>
+      </c>
+      <c r="S53" t="n">
+        <v>59705057.6002043</v>
+      </c>
+      <c r="T53" t="n">
+        <v>42486481.0119743</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B54" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C54" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D54" t="n">
         <v>30</v>
       </c>
       <c r="E54" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F54" t="n">
         <v>35165797.2154787</v>
@@ -2870,22 +3689,37 @@
       <c r="O54" t="n">
         <v>0.016496070124398</v>
       </c>
+      <c r="P54" t="n">
+        <v>35165797.2154787</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>30</v>
+      </c>
+      <c r="R54" t="n">
+        <v>10382102.901732</v>
+      </c>
+      <c r="S54" t="n">
+        <v>59949491.5292254</v>
+      </c>
+      <c r="T54" t="n">
+        <v>35165797.2154787</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B55" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C55" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D55" t="n">
         <v>6</v>
       </c>
       <c r="E55" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F55" t="n">
         <v>350135.034247371</v>
@@ -2915,22 +3749,37 @@
       <c r="O55" t="n">
         <v>0.773293575326175</v>
       </c>
+      <c r="P55" t="n">
+        <v>350135.034247371</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>30</v>
+      </c>
+      <c r="R55" t="n">
+        <v>-2033239.80329576</v>
+      </c>
+      <c r="S55" t="n">
+        <v>2733509.8717905</v>
+      </c>
+      <c r="T55" t="n">
+        <v>350135.034247371</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B56" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D56" t="n">
         <v>20</v>
       </c>
       <c r="E56" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F56" t="n">
         <v>3263879.12351651</v>
@@ -2960,22 +3809,37 @@
       <c r="O56" t="n">
         <v>0.0469677779015308</v>
       </c>
+      <c r="P56" t="n">
+        <v>3263879.12351651</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>30</v>
+      </c>
+      <c r="R56" t="n">
+        <v>532959.281026562</v>
+      </c>
+      <c r="S56" t="n">
+        <v>5994798.96600646</v>
+      </c>
+      <c r="T56" t="n">
+        <v>3263879.12351651</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B57" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C57" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D57" t="n">
         <v>22</v>
       </c>
       <c r="E57" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F57" t="n">
         <v>11713398.8778617</v>
@@ -3005,22 +3869,37 @@
       <c r="O57" t="n">
         <v>0.0000787293470095358</v>
       </c>
+      <c r="P57" t="n">
+        <v>11713398.8778617</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>30</v>
+      </c>
+      <c r="R57" t="n">
+        <v>7364754.37105483</v>
+      </c>
+      <c r="S57" t="n">
+        <v>16062043.3846686</v>
+      </c>
+      <c r="T57" t="n">
+        <v>11713398.8778617</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D58" t="n">
         <v>28</v>
       </c>
       <c r="E58" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F58" t="n">
         <v>0.932722405818427</v>
@@ -3048,22 +3927,37 @@
       <c r="O58" t="n">
         <v>0.011258480469007</v>
       </c>
+      <c r="P58" t="n">
+        <v>2.54141854092791</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>44</v>
+      </c>
+      <c r="R58" t="n">
+        <v>1.33133591380296</v>
+      </c>
+      <c r="S58" t="n">
+        <v>4.85137382174463</v>
+      </c>
+      <c r="T58" t="n">
+        <v>1.54141854092791</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B59" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C59" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D59" t="n">
         <v>5</v>
       </c>
       <c r="E59" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F59" t="n">
         <v>-1.73028397069876</v>
@@ -3091,22 +3985,37 @@
       <c r="O59" t="n">
         <v>0.929847594852328</v>
       </c>
+      <c r="P59" t="n">
+        <v>0.177234073539473</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>44</v>
+      </c>
+      <c r="R59" t="n">
+        <v>0.000677332374904566</v>
+      </c>
+      <c r="S59" t="n">
+        <v>46.375927073944</v>
+      </c>
+      <c r="T59" t="n">
+        <v>-0.822765926460527</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C60" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D60" t="n">
         <v>18</v>
       </c>
       <c r="E60" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F60" t="n">
         <v>-0.316511882895824</v>
@@ -3134,22 +4043,37 @@
       <c r="O60" t="n">
         <v>0.940086873939304</v>
       </c>
+      <c r="P60" t="n">
+        <v>0.728686352604321</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>44</v>
+      </c>
+      <c r="R60" t="n">
+        <v>0.0791545086913871</v>
+      </c>
+      <c r="S60" t="n">
+        <v>6.70819400246706</v>
+      </c>
+      <c r="T60" t="n">
+        <v>-0.271313647395679</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B61" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C61" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D61" t="n">
         <v>20</v>
       </c>
       <c r="E61" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F61" t="n">
         <v>1.65854360719484</v>
@@ -3177,22 +4101,37 @@
       <c r="O61" t="n">
         <v>0.0108276651560904</v>
       </c>
+      <c r="P61" t="n">
+        <v>5.25165679697568</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>44</v>
+      </c>
+      <c r="R61" t="n">
+        <v>1.71881949267503</v>
+      </c>
+      <c r="S61" t="n">
+        <v>16.0458379898275</v>
+      </c>
+      <c r="T61" t="n">
+        <v>4.25165679697568</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D62" t="n">
         <v>28</v>
       </c>
       <c r="E62" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F62" t="n">
         <v>67.6911411411156</v>
@@ -3220,22 +4159,37 @@
       <c r="O62" t="n">
         <v>0.476961662165376</v>
       </c>
+      <c r="P62" t="n">
+        <v>249970679823008484921318572032</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>44</v>
+      </c>
+      <c r="R62" t="n">
+        <v>0.0000000000000000000329893405932909</v>
+      </c>
+      <c r="S62" t="n">
+        <v>1894106994787450506365713689185250922377344184350400589517364772697850867875840</v>
+      </c>
+      <c r="T62" t="n">
+        <v>249970679823008484921318572032</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B63" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C63" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D63" t="n">
         <v>6</v>
       </c>
       <c r="E63" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F63" t="n">
         <v>22.1933943083372</v>
@@ -3263,22 +4217,37 @@
       <c r="O63" t="n">
         <v>0.940086873939304</v>
       </c>
+      <c r="P63" t="n">
+        <v>4349793929.24356</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>44</v>
+      </c>
+      <c r="R63" t="n">
+        <v>1.9780419993743e-242</v>
+      </c>
+      <c r="S63" t="n">
+        <v>9.56537183379878e+260</v>
+      </c>
+      <c r="T63" t="n">
+        <v>4349793928.24356</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B64" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C64" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D64" t="n">
         <v>19</v>
       </c>
       <c r="E64" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F64" t="n">
         <v>-73.6052800188648</v>
@@ -3306,22 +4275,37 @@
       <c r="O64" t="n">
         <v>0.940086873939304</v>
       </c>
+      <c r="P64" t="n">
+        <v>0.000000000000000000000000000000010805205945045</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>44</v>
+      </c>
+      <c r="R64" t="n">
+        <v>0</v>
+      </c>
+      <c r="S64" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="T64" t="n">
+        <v>-1</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B65" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D65" t="n">
         <v>21</v>
       </c>
       <c r="E65" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F65" t="n">
         <v>68.2472352272114</v>
@@ -3349,22 +4333,37 @@
       <c r="O65" t="n">
         <v>0.940086873939304</v>
       </c>
+      <c r="P65" t="n">
+        <v>435910835356686171764384858112</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>44</v>
+      </c>
+      <c r="R65" t="n">
+        <v>0</v>
+      </c>
+      <c r="S65" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="T65" t="n">
+        <v>435910835356686171764384858112</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B66" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C66" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D66" t="n">
         <v>28</v>
       </c>
       <c r="E66" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F66" t="n">
         <v>0.000568911687166622</v>
@@ -3392,22 +4391,37 @@
       <c r="O66" t="n">
         <v>0.00789314679012567</v>
       </c>
+      <c r="P66" t="n">
+        <v>1.00056907354811</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>44</v>
+      </c>
+      <c r="R66" t="n">
+        <v>1.00022184784466</v>
+      </c>
+      <c r="S66" t="n">
+        <v>1.00091641979051</v>
+      </c>
+      <c r="T66" t="n">
+        <v>0.000569073548113863</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B67" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C67" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D67" t="n">
         <v>6</v>
       </c>
       <c r="E67" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F67" t="n">
         <v>0.0107394832014028</v>
@@ -3435,22 +4449,37 @@
       <c r="O67" t="n">
         <v>0.940086873939304</v>
       </c>
+      <c r="P67" t="n">
+        <v>1.01079735844898</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>44</v>
+      </c>
+      <c r="R67" t="n">
+        <v>0.952706150946862</v>
+      </c>
+      <c r="S67" t="n">
+        <v>1.07243067427664</v>
+      </c>
+      <c r="T67" t="n">
+        <v>0.0107973584489829</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B68" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C68" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D68" t="n">
         <v>19</v>
       </c>
       <c r="E68" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F68" t="n">
         <v>0.0029562398725963</v>
@@ -3478,22 +4507,37 @@
       <c r="O68" t="n">
         <v>0.0108276651560904</v>
       </c>
+      <c r="P68" t="n">
+        <v>1.00296061385881</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>44</v>
+      </c>
+      <c r="R68" t="n">
+        <v>1.00102095609885</v>
+      </c>
+      <c r="S68" t="n">
+        <v>1.0049040300538</v>
+      </c>
+      <c r="T68" t="n">
+        <v>0.00296061385881052</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B69" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C69" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D69" t="n">
         <v>21</v>
       </c>
       <c r="E69" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F69" t="n">
         <v>0.00339025060356143</v>
@@ -3520,6 +4564,21 @@
       <c r="N69"/>
       <c r="O69" t="n">
         <v>0.0000000000000034516033329981</v>
+      </c>
+      <c r="P69" t="n">
+        <v>1.00339600400312</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>44</v>
+      </c>
+      <c r="R69" t="n">
+        <v>1.00258109820283</v>
+      </c>
+      <c r="S69" t="n">
+        <v>1.00421157216526</v>
+      </c>
+      <c r="T69" t="n">
+        <v>0.00339600400312379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>